<commit_message>
refatorei os codigos de segmentacao, rfma, faturamento e metricas de recorrencia e retencao para bibi
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/metricas_recorrencia_anual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/metricas_recorrencia_anual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>ano</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>returning_rate</t>
+  </si>
+  <si>
+    <t>2021</t>
   </si>
   <si>
     <t>2022</t>
@@ -407,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,22 +450,22 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>362</v>
+        <v>485</v>
       </c>
       <c r="D2">
-        <v>167</v>
+        <v>66</v>
       </c>
       <c r="E2">
-        <v>195</v>
+        <v>419</v>
       </c>
       <c r="F2">
-        <v>35.0104821802935</v>
+        <v>60.55045871559633</v>
       </c>
       <c r="G2">
-        <v>53.86740331491713</v>
+        <v>86.39175257731959</v>
       </c>
       <c r="H2">
-        <v>46.13259668508287</v>
+        <v>13.60824742268041</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -473,22 +476,22 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>320</v>
+        <v>362</v>
       </c>
       <c r="D3">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="E3">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="F3">
-        <v>51.38121546961326</v>
+        <v>34.43298969072165</v>
       </c>
       <c r="G3">
-        <v>41.875</v>
+        <v>53.86740331491713</v>
       </c>
       <c r="H3">
-        <v>58.12500000000001</v>
+        <v>46.13259668508287</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -499,22 +502,22 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>457</v>
+        <v>320</v>
       </c>
       <c r="D4">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="E4">
-        <v>224</v>
+        <v>134</v>
       </c>
       <c r="F4">
-        <v>72.8125</v>
+        <v>51.38121546961326</v>
       </c>
       <c r="G4">
-        <v>49.01531728665208</v>
+        <v>41.875</v>
       </c>
       <c r="H4">
-        <v>50.98468271334792</v>
+        <v>58.12500000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -525,22 +528,48 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>298</v>
+        <v>457</v>
       </c>
       <c r="D5">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>224</v>
       </c>
       <c r="F5">
-        <v>59.08096280087527</v>
+        <v>72.8125</v>
       </c>
       <c r="G5">
-        <v>9.395973154362416</v>
+        <v>49.01531728665208</v>
       </c>
       <c r="H5">
-        <v>90.60402684563759</v>
+        <v>50.98468271334792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>340</v>
+      </c>
+      <c r="D6">
+        <v>290</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>63.45733041575492</v>
+      </c>
+      <c r="G6">
+        <v>14.70588235294118</v>
+      </c>
+      <c r="H6">
+        <v>85.29411764705883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>